<commit_message>
Se incluyo numero de doc. retenciones_declaradas_sin_cruzar_en_profit
</commit_message>
<xml_diff>
--- a/diferencias_cruce.xlsx
+++ b/diferencias_cruce.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N73"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3038,17 +3038,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t xml:space="preserve">656             </t>
+          <t xml:space="preserve">654             </t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>J308226505</t>
+          <t>J308226440</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
+          <t>SUPERMERCADO LA MANSION DEL CARIBE C.A</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -3058,33 +3058,33 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>9800</t>
+          <t>9799</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>00-00011141</t>
+          <t>00-00011140</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>00-00011141</t>
+          <t>00-00011140</t>
         </is>
       </c>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000614          </t>
+          <t xml:space="preserve">0000000821          </t>
         </is>
       </c>
       <c r="K44" t="n">
-        <v>947.21</v>
+        <v>1488.31</v>
       </c>
       <c r="L44" t="n">
-        <v>946.37</v>
+        <v>1487.84</v>
       </c>
       <c r="M44" t="n">
-        <v>0.84</v>
+        <v>0.47</v>
       </c>
       <c r="N44" t="inlineStr">
         <is>
@@ -3098,53 +3098,53 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t xml:space="preserve">656             </t>
+          <t xml:space="preserve">654             </t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>J308226505</t>
+          <t>J308226440</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
+          <t>SUPERMERCADO LA MANSION DEL CARIBE C.A</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>04-10-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>9894</t>
+          <t>10011</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>00-00011235</t>
+          <t>00-00011352</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>00-00011235</t>
+          <t>00-00011352</t>
         </is>
       </c>
       <c r="I45" t="inlineStr"/>
       <c r="J45" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000616          </t>
+          <t xml:space="preserve">0000000820          </t>
         </is>
       </c>
       <c r="K45" t="n">
-        <v>179.8</v>
+        <v>261.32</v>
       </c>
       <c r="L45" t="n">
-        <v>179.77</v>
+        <v>260.91</v>
       </c>
       <c r="M45" t="n">
-        <v>0.03</v>
+        <v>0.41</v>
       </c>
       <c r="N45" t="inlineStr">
         <is>
@@ -3158,53 +3158,53 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t xml:space="preserve">656             </t>
+          <t xml:space="preserve">654             </t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>J308226505</t>
+          <t>J308226440</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
+          <t>SUPERMERCADO LA MANSION DEL CARIBE C.A</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>08-10-2024</t>
+          <t>15-10-2024</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>9948</t>
+          <t>10075</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>00-00011289</t>
+          <t>00-00011416</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>00-00011289</t>
+          <t>00-00011416</t>
         </is>
       </c>
       <c r="I46" t="inlineStr"/>
       <c r="J46" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000615          </t>
+          <t xml:space="preserve">0000000822          </t>
         </is>
       </c>
       <c r="K46" t="n">
-        <v>285.35</v>
+        <v>105.03</v>
       </c>
       <c r="L46" t="n">
-        <v>285.21</v>
+        <v>105</v>
       </c>
       <c r="M46" t="n">
-        <v>0.14</v>
+        <v>0.03</v>
       </c>
       <c r="N46" t="inlineStr">
         <is>
@@ -3218,17 +3218,17 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t xml:space="preserve">833             </t>
+          <t xml:space="preserve">656             </t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>J308445240</t>
+          <t>J308226505</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>CORPORACION BAGATELLE, C.A.</t>
+          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -3238,33 +3238,33 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>9818</t>
+          <t>9800</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>00-00011159</t>
+          <t>00-00011141</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>00-00011159</t>
+          <t>00-00011141</t>
         </is>
       </c>
       <c r="I47" t="inlineStr"/>
       <c r="J47" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000426          </t>
+          <t xml:space="preserve">0000000614          </t>
         </is>
       </c>
       <c r="K47" t="n">
-        <v>715.1799999999999</v>
+        <v>947.21</v>
       </c>
       <c r="L47" t="n">
-        <v>714.95</v>
+        <v>946.37</v>
       </c>
       <c r="M47" t="n">
-        <v>0.23</v>
+        <v>0.84</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
@@ -3278,53 +3278,53 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t xml:space="preserve">833             </t>
+          <t xml:space="preserve">656             </t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>J308445240</t>
+          <t>J308226505</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>CORPORACION BAGATELLE, C.A.</t>
+          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>01-10-2024</t>
+          <t>04-10-2024</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>9820</t>
+          <t>9894</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>00-00011161</t>
+          <t>00-00011235</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>00-00011161</t>
+          <t>00-00011235</t>
         </is>
       </c>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000427          </t>
+          <t xml:space="preserve">0000000616          </t>
         </is>
       </c>
       <c r="K48" t="n">
-        <v>453.56</v>
+        <v>179.8</v>
       </c>
       <c r="L48" t="n">
-        <v>453.25</v>
+        <v>179.77</v>
       </c>
       <c r="M48" t="n">
-        <v>0.31</v>
+        <v>0.03</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
@@ -3338,53 +3338,53 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t xml:space="preserve">833             </t>
+          <t xml:space="preserve">656             </t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>J308445240</t>
+          <t>J308226505</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>CORPORACION BAGATELLE, C.A.</t>
+          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>01-10-2024</t>
+          <t>08-10-2024</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>9821</t>
+          <t>9948</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>00-00011162</t>
+          <t>00-00011289</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>00-00011162</t>
+          <t>00-00011289</t>
         </is>
       </c>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000428          </t>
+          <t xml:space="preserve">0000000615          </t>
         </is>
       </c>
       <c r="K49" t="n">
-        <v>663.08</v>
+        <v>285.35</v>
       </c>
       <c r="L49" t="n">
-        <v>662.9</v>
+        <v>285.21</v>
       </c>
       <c r="M49" t="n">
-        <v>0.18</v>
+        <v>0.14</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>
@@ -3398,57 +3398,57 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t xml:space="preserve">833             </t>
+          <t xml:space="preserve">656             </t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>J308445240</t>
+          <t>J308226505</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>CORPORACION BAGATELLE, C.A.</t>
+          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>01-10-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>9822</t>
+          <t>10012</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>00-00011163</t>
+          <t>00-00011353</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>00-00011163</t>
+          <t>00-00011353</t>
         </is>
       </c>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000429          </t>
+          <t xml:space="preserve">0000000825          </t>
         </is>
       </c>
       <c r="K50" t="n">
-        <v>119.62</v>
+        <v>555.71</v>
       </c>
       <c r="L50" t="n">
-        <v>119.59</v>
+        <v>555.71</v>
       </c>
       <c r="M50" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -3458,57 +3458,57 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t xml:space="preserve">833             </t>
+          <t xml:space="preserve">656             </t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>J308445240</t>
+          <t>J308226505</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>CORPORACION BAGATELLE, C.A.</t>
+          <t>PANADERIA Y PASTELERIA LA MANSION DEL CARIBE C.A.</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>04-10-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>9905</t>
+          <t>10013</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>00-00011246</t>
+          <t>00-00011354</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>00-00011246</t>
+          <t>00-00011354</t>
         </is>
       </c>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000491          </t>
+          <t xml:space="preserve">0000000826          </t>
         </is>
       </c>
       <c r="K51" t="n">
-        <v>355.52</v>
+        <v>977.5700000000001</v>
       </c>
       <c r="L51" t="n">
-        <v>355.47</v>
+        <v>977.77</v>
       </c>
       <c r="M51" t="n">
-        <v>0.05</v>
+        <v>-0.2</v>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -3533,42 +3533,42 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>04-10-2024</t>
+          <t>01-10-2024</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>9906</t>
+          <t>9818</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>00-00011247</t>
+          <t>00-00011159</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>00-00011247</t>
+          <t>00-00011159</t>
         </is>
       </c>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000490          </t>
+          <t xml:space="preserve">0000000426          </t>
         </is>
       </c>
       <c r="K52" t="n">
-        <v>119.85</v>
+        <v>715.1799999999999</v>
       </c>
       <c r="L52" t="n">
-        <v>119.85</v>
+        <v>714.95</v>
       </c>
       <c r="M52" t="n">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -3593,38 +3593,38 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>07-10-2024</t>
+          <t>01-10-2024</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>9944</t>
+          <t>9820</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>00-00011285</t>
+          <t>00-00011161</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>00-00011285</t>
+          <t>00-00011161</t>
         </is>
       </c>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000489          </t>
+          <t xml:space="preserve">0000000427          </t>
         </is>
       </c>
       <c r="K53" t="n">
-        <v>316</v>
+        <v>453.56</v>
       </c>
       <c r="L53" t="n">
-        <v>315.95</v>
+        <v>453.25</v>
       </c>
       <c r="M53" t="n">
-        <v>0.05</v>
+        <v>0.31</v>
       </c>
       <c r="N53" t="inlineStr">
         <is>
@@ -3638,17 +3638,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t xml:space="preserve">539             </t>
+          <t xml:space="preserve">833             </t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>J309277367</t>
+          <t>J308445240</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
+          <t>CORPORACION BAGATELLE, C.A.</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -3658,37 +3658,37 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>9798</t>
+          <t>9821</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>00-00011139</t>
+          <t>00-00011162</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>00-00011139</t>
+          <t>00-00011162</t>
         </is>
       </c>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000577          </t>
+          <t xml:space="preserve">0000000428          </t>
         </is>
       </c>
       <c r="K54" t="n">
-        <v>804.08</v>
+        <v>663.08</v>
       </c>
       <c r="L54" t="n">
-        <v>804.27</v>
+        <v>662.9</v>
       </c>
       <c r="M54" t="n">
-        <v>-0.19</v>
+        <v>0.18</v>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -3698,57 +3698,57 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t xml:space="preserve">539             </t>
+          <t xml:space="preserve">833             </t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>J309277367</t>
+          <t>J308445240</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
+          <t>CORPORACION BAGATELLE, C.A.</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>04-10-2024</t>
+          <t>01-10-2024</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>9891</t>
+          <t>9822</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>00-00011232</t>
+          <t>00-00011163</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>00-00011232</t>
+          <t>00-00011163</t>
         </is>
       </c>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000578          </t>
+          <t xml:space="preserve">0000000429          </t>
         </is>
       </c>
       <c r="K55" t="n">
-        <v>239.69</v>
+        <v>119.62</v>
       </c>
       <c r="L55" t="n">
-        <v>239.7</v>
+        <v>119.59</v>
       </c>
       <c r="M55" t="n">
-        <v>-0.01</v>
+        <v>0.03</v>
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -3758,57 +3758,57 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t xml:space="preserve">539             </t>
+          <t xml:space="preserve">833             </t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>J309277367</t>
+          <t>J308445240</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
+          <t>CORPORACION BAGATELLE, C.A.</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>08-10-2024</t>
+          <t>04-10-2024</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>9947</t>
+          <t>9905</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>00-00011288</t>
+          <t>00-00011246</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>00-00011288</t>
+          <t>00-00011246</t>
         </is>
       </c>
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000580          </t>
+          <t xml:space="preserve">0000000491          </t>
         </is>
       </c>
       <c r="K56" t="n">
-        <v>837.8099999999999</v>
+        <v>355.52</v>
       </c>
       <c r="L56" t="n">
-        <v>837.84</v>
+        <v>355.47</v>
       </c>
       <c r="M56" t="n">
-        <v>-0.03</v>
+        <v>0.05</v>
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -3818,57 +3818,57 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t xml:space="preserve">539             </t>
+          <t xml:space="preserve">833             </t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>J309277367</t>
+          <t>J308445240</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
+          <t>CORPORACION BAGATELLE, C.A.</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>11-10-2024</t>
+          <t>04-10-2024</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>10051</t>
+          <t>9906</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>00-00011392</t>
+          <t>00-00011247</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>00-00011392</t>
+          <t>00-00011247</t>
         </is>
       </c>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000596          </t>
+          <t xml:space="preserve">0000000490          </t>
         </is>
       </c>
       <c r="K57" t="n">
-        <v>641.49</v>
+        <v>119.85</v>
       </c>
       <c r="L57" t="n">
-        <v>641.1799999999999</v>
+        <v>119.85</v>
       </c>
       <c r="M57" t="n">
-        <v>0.31</v>
+        <v>0</v>
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -3878,59 +3878,57 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t xml:space="preserve">856             </t>
+          <t xml:space="preserve">833             </t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>J310438030</t>
+          <t>J308445240</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA EL ANTOJITO, C.A.</t>
+          <t>CORPORACION BAGATELLE, C.A.</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>03-10-2024</t>
+          <t>07-10-2024</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>9870</t>
+          <t>9944</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>00-00011211</t>
-        </is>
-      </c>
-      <c r="H58" t="n">
-        <v>11211</v>
-      </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>verificar n.control</t>
-        </is>
-      </c>
+          <t>00-00011285</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>00-00011285</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr"/>
       <c r="J58" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000629          </t>
+          <t xml:space="preserve">0000000489          </t>
         </is>
       </c>
       <c r="K58" t="n">
-        <v>216.79</v>
+        <v>316</v>
       </c>
       <c r="L58" t="n">
-        <v>217.07</v>
+        <v>315.95</v>
       </c>
       <c r="M58" t="n">
-        <v>-0.28</v>
+        <v>0.05</v>
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -3940,57 +3938,57 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t xml:space="preserve">607             </t>
+          <t xml:space="preserve">539             </t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>J311906371</t>
+          <t>J309277367</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>PASTELERIA LA TRUFA C.A</t>
+          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>26-09-2024</t>
+          <t>01-10-2024</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>9721</t>
+          <t>9798</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>00-00011062</t>
+          <t>00-00011139</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>00-00011062</t>
+          <t>00-00011139</t>
         </is>
       </c>
       <c r="I59" t="inlineStr"/>
       <c r="J59" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000361          </t>
+          <t xml:space="preserve">0000000577          </t>
         </is>
       </c>
       <c r="K59" t="n">
-        <v>587.36</v>
+        <v>804.08</v>
       </c>
       <c r="L59" t="n">
-        <v>440.73</v>
+        <v>804.27</v>
       </c>
       <c r="M59" t="n">
-        <v>146.63</v>
+        <v>-0.19</v>
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -4000,53 +3998,53 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t xml:space="preserve">607             </t>
+          <t xml:space="preserve">539             </t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>J311906371</t>
+          <t>J309277367</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>PASTELERIA LA TRUFA C.A</t>
+          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>10-10-2024</t>
+          <t>04-10-2024</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>9997</t>
+          <t>9891</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>00-00011338</t>
+          <t>00-00011232</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>00-00011338</t>
+          <t>00-00011232</t>
         </is>
       </c>
       <c r="I60" t="inlineStr"/>
       <c r="J60" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000626          </t>
+          <t xml:space="preserve">0000000578          </t>
         </is>
       </c>
       <c r="K60" t="n">
-        <v>40.53</v>
+        <v>239.69</v>
       </c>
       <c r="L60" t="n">
-        <v>40.53</v>
+        <v>239.7</v>
       </c>
       <c r="M60" t="n">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="N60" t="inlineStr">
         <is>
@@ -4060,57 +4058,57 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t xml:space="preserve">626             </t>
+          <t xml:space="preserve">539             </t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>J313156450</t>
+          <t>J309277367</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>PANADERIA PASTELERIA FLOR DEL AVILA 24.18, C.A.</t>
+          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>02-10-2024</t>
+          <t>08-10-2024</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>9849</t>
+          <t>9947</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>00-00011190</t>
+          <t>00-00011288</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>00-00011190</t>
+          <t>00-00011288</t>
         </is>
       </c>
       <c r="I61" t="inlineStr"/>
       <c r="J61" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000606          </t>
+          <t xml:space="preserve">0000000580          </t>
         </is>
       </c>
       <c r="K61" t="n">
-        <v>164.81</v>
+        <v>837.8099999999999</v>
       </c>
       <c r="L61" t="n">
-        <v>164.66</v>
+        <v>837.84</v>
       </c>
       <c r="M61" t="n">
-        <v>0.15</v>
+        <v>-0.03</v>
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -4120,17 +4118,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t xml:space="preserve">626             </t>
+          <t xml:space="preserve">539             </t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>J313156450</t>
+          <t>J309277367</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>PANADERIA PASTELERIA FLOR DEL AVILA 24.18, C.A.</t>
+          <t>PANADERIA Y PASTELERIA EL SIGLO DEL PAN C.A.</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -4140,37 +4138,37 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>10042</t>
+          <t>10051</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>00-00011383</t>
+          <t>00-00011392</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>00-00011383</t>
+          <t>00-00011392</t>
         </is>
       </c>
       <c r="I62" t="inlineStr"/>
       <c r="J62" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000605          </t>
+          <t xml:space="preserve">0000000596          </t>
         </is>
       </c>
       <c r="K62" t="n">
-        <v>116.32</v>
+        <v>641.49</v>
       </c>
       <c r="L62" t="n">
-        <v>116.34</v>
+        <v>641.1799999999999</v>
       </c>
       <c r="M62" t="n">
-        <v>-0.02</v>
+        <v>0.31</v>
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -4180,36 +4178,36 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t xml:space="preserve">031             </t>
+          <t xml:space="preserve">856             </t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>J315313693</t>
+          <t>J310438030</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
+          <t>PANADERIA Y PASTELERIA EL ANTOJITO, C.A.</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>01-10-2024</t>
+          <t>03-10-2024</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>9802</t>
+          <t>9870</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>00-00011143</t>
+          <t>00-00011211</t>
         </is>
       </c>
       <c r="H63" t="n">
-        <v>11143</v>
+        <v>11211</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
@@ -4218,17 +4216,17 @@
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000476          </t>
+          <t xml:space="preserve">0000000629          </t>
         </is>
       </c>
       <c r="K63" t="n">
-        <v>525.45</v>
+        <v>216.79</v>
       </c>
       <c r="L63" t="n">
-        <v>525.6</v>
+        <v>217.07</v>
       </c>
       <c r="M63" t="n">
-        <v>-0.15</v>
+        <v>-0.28</v>
       </c>
       <c r="N63" t="inlineStr">
         <is>
@@ -4242,59 +4240,57 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t xml:space="preserve">031             </t>
+          <t xml:space="preserve">607             </t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>J315313693</t>
+          <t>J311906371</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
+          <t>PASTELERIA LA TRUFA C.A</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>04-10-2024</t>
+          <t>26-09-2024</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>9898</t>
+          <t>9721</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>00-00011239</t>
-        </is>
-      </c>
-      <c r="H64" t="n">
-        <v>11239</v>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>verificar n.control</t>
-        </is>
-      </c>
+          <t>00-00011062</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>00-00011062</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr"/>
       <c r="J64" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000742          </t>
+          <t xml:space="preserve">0000000361          </t>
         </is>
       </c>
       <c r="K64" t="n">
-        <v>229.22</v>
+        <v>587.36</v>
       </c>
       <c r="L64" t="n">
-        <v>229.34</v>
+        <v>440.73</v>
       </c>
       <c r="M64" t="n">
-        <v>-0.12</v>
+        <v>146.63</v>
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -4304,59 +4300,57 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t xml:space="preserve">031             </t>
+          <t xml:space="preserve">607             </t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>J315313693</t>
+          <t>J311906371</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
+          <t>PASTELERIA LA TRUFA C.A</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>07-10-2024</t>
+          <t>10-10-2024</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>9930</t>
+          <t>9997</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>00-00011271</t>
-        </is>
-      </c>
-      <c r="H65" t="n">
-        <v>11271</v>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>verificar n.control</t>
-        </is>
-      </c>
+          <t>00-00011338</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>00-00011338</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr"/>
       <c r="J65" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000743          </t>
+          <t xml:space="preserve">0000000626          </t>
         </is>
       </c>
       <c r="K65" t="n">
-        <v>375.72</v>
+        <v>40.53</v>
       </c>
       <c r="L65" t="n">
-        <v>375.59</v>
+        <v>40.53</v>
       </c>
       <c r="M65" t="n">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -4366,55 +4360,53 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t xml:space="preserve">031             </t>
+          <t xml:space="preserve">626             </t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>J315313693</t>
+          <t>J313156450</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
+          <t>PANADERIA PASTELERIA FLOR DEL AVILA 24.18, C.A.</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>11-10-2024</t>
+          <t>02-10-2024</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>10019</t>
+          <t>9849</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>00-00011360</t>
-        </is>
-      </c>
-      <c r="H66" t="n">
-        <v>11360</v>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>verificar n.control</t>
-        </is>
-      </c>
+          <t>00-00011190</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>00-00011190</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr"/>
       <c r="J66" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000744          </t>
+          <t xml:space="preserve">0000000606          </t>
         </is>
       </c>
       <c r="K66" t="n">
-        <v>279.03</v>
+        <v>164.81</v>
       </c>
       <c r="L66" t="n">
-        <v>278.99</v>
+        <v>164.66</v>
       </c>
       <c r="M66" t="n">
-        <v>0.04</v>
+        <v>0.15</v>
       </c>
       <c r="N66" t="inlineStr">
         <is>
@@ -4428,17 +4420,17 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t xml:space="preserve">653             </t>
+          <t xml:space="preserve">626             </t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>J401041710</t>
+          <t>J313156450</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>INVERSIONES DOÑA ROSA 72 C. A</t>
+          <t>PANADERIA PASTELERIA FLOR DEL AVILA 24.18, C.A.</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -4448,33 +4440,33 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>10018</t>
+          <t>10042</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>00-00011359</t>
+          <t>00-00011383</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>00-00011359</t>
+          <t>00-00011383</t>
         </is>
       </c>
       <c r="I67" t="inlineStr"/>
       <c r="J67" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000775          </t>
+          <t xml:space="preserve">0000000605          </t>
         </is>
       </c>
       <c r="K67" t="n">
-        <v>1217.6</v>
+        <v>116.32</v>
       </c>
       <c r="L67" t="n">
-        <v>1217.6</v>
+        <v>116.34</v>
       </c>
       <c r="M67" t="n">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
       <c r="N67" t="inlineStr">
         <is>
@@ -4488,36 +4480,36 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t xml:space="preserve">862             </t>
+          <t xml:space="preserve">031             </t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>J402111991</t>
+          <t>J315313693</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>PIU EXPRESS, C.A.</t>
+          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>10-10-2024</t>
+          <t>01-10-2024</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>10002</t>
+          <t>9802</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>00-00011343</t>
+          <t>00-00011143</t>
         </is>
       </c>
       <c r="H68" t="n">
-        <v>11343</v>
+        <v>11143</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
@@ -4526,21 +4518,21 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000633          </t>
+          <t xml:space="preserve">0000000476          </t>
         </is>
       </c>
       <c r="K68" t="n">
-        <v>699.3099999999999</v>
+        <v>525.45</v>
       </c>
       <c r="L68" t="n">
-        <v>699.1799999999999</v>
+        <v>525.6</v>
       </c>
       <c r="M68" t="n">
-        <v>0.13</v>
+        <v>-0.15</v>
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -4550,57 +4542,59 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t xml:space="preserve">854             </t>
+          <t xml:space="preserve">031             </t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>J405522194</t>
+          <t>J315313693</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>CAFE EUROPA 2015, C.A.</t>
+          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>03-10-2024</t>
+          <t>04-10-2024</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>9867</t>
+          <t>9898</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>00-00011208</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>00-00011208</t>
-        </is>
-      </c>
-      <c r="I69" t="inlineStr"/>
+          <t>00-00011239</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>11239</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>verificar n.control</t>
+        </is>
+      </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000407          </t>
+          <t xml:space="preserve">0000000742          </t>
         </is>
       </c>
       <c r="K69" t="n">
-        <v>119.82</v>
+        <v>229.22</v>
       </c>
       <c r="L69" t="n">
-        <v>89.86</v>
+        <v>229.34</v>
       </c>
       <c r="M69" t="n">
-        <v>29.96</v>
+        <v>-0.12</v>
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -4610,57 +4604,59 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t xml:space="preserve">566             </t>
+          <t xml:space="preserve">031             </t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>J406284513</t>
+          <t>J315313693</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>NOSSO CAFE, C.A.</t>
+          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>11-10-2024</t>
+          <t>07-10-2024</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>10027</t>
+          <t>9930</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>00-00011368</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>00-00011368</t>
-        </is>
-      </c>
-      <c r="I70" t="inlineStr"/>
+          <t>00-00011271</t>
+        </is>
+      </c>
+      <c r="H70" t="n">
+        <v>11271</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>verificar n.control</t>
+        </is>
+      </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000463          </t>
+          <t xml:space="preserve">0000000743          </t>
         </is>
       </c>
       <c r="K70" t="n">
-        <v>121.99</v>
+        <v>375.72</v>
       </c>
       <c r="L70" t="n">
-        <v>121.99</v>
+        <v>375.59</v>
       </c>
       <c r="M70" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -4670,57 +4666,59 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t xml:space="preserve">848             </t>
+          <t xml:space="preserve">031             </t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>J500533993</t>
+          <t>J315313693</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>PANADERIA Y PASTELERIA TROPICAL PAN, C.A.</t>
+          <t>INVERSIONES MANUEL PEREIRA , C.A.</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>14-10-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>10067</t>
+          <t>10019</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>00-00011408</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>00-00011408</t>
-        </is>
-      </c>
-      <c r="I71" t="inlineStr"/>
+          <t>00-00011360</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>11360</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>verificar n.control</t>
+        </is>
+      </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000750          </t>
+          <t xml:space="preserve">0000000744          </t>
         </is>
       </c>
       <c r="K71" t="n">
-        <v>722.96</v>
+        <v>279.03</v>
       </c>
       <c r="L71" t="n">
-        <v>722.97</v>
+        <v>278.99</v>
       </c>
       <c r="M71" t="n">
-        <v>-0.01</v>
+        <v>0.04</v>
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>(-) de menos</t>
+          <t>(+) de más</t>
         </is>
       </c>
     </row>
@@ -4730,57 +4728,57 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t xml:space="preserve">860             </t>
+          <t xml:space="preserve">653             </t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>J500705050</t>
+          <t>J401041710</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>INVERSIONES REGALEIRA, C.A.</t>
+          <t>INVERSIONES DOÑA ROSA 72 C. A</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>30-09-2024</t>
+          <t>04-10-2024</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>9773</t>
+          <t>9893</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>00-00011114</t>
+          <t>00-00011234</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>00-00011114</t>
+          <t>00-00011234</t>
         </is>
       </c>
       <c r="I72" t="inlineStr"/>
       <c r="J72" t="inlineStr">
         <is>
-          <t xml:space="preserve">0000000497          </t>
+          <t xml:space="preserve">0000000827          </t>
         </is>
       </c>
       <c r="K72" t="n">
-        <v>433.7</v>
+        <v>1572.99</v>
       </c>
       <c r="L72" t="n">
-        <v>325.18</v>
+        <v>1573.18</v>
       </c>
       <c r="M72" t="n">
-        <v>108.52</v>
+        <v>-0.19</v>
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>(+) de más</t>
+          <t>(-) de menos</t>
         </is>
       </c>
     </row>
@@ -4790,57 +4788,539 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t xml:space="preserve">653             </t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>J401041710</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>INVERSIONES DOÑA ROSA 72 C. A</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>10008</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>00-00011349</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>00-00011349</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000818          </t>
+        </is>
+      </c>
+      <c r="K73" t="n">
+        <v>467.33</v>
+      </c>
+      <c r="L73" t="n">
+        <v>467.24</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>(+) de más</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">653             </t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>J401041710</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>INVERSIONES DOÑA ROSA 72 C. A</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>10018</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>00-00011359</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>00-00011359</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000775          </t>
+        </is>
+      </c>
+      <c r="K74" t="n">
+        <v>1217.6</v>
+      </c>
+      <c r="L74" t="n">
+        <v>1217.6</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>(-) de menos</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">653             </t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>J401041710</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>INVERSIONES DOÑA ROSA 72 C. A</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>15-10-2024</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>10078</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>00-00011419</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>00-00011419</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000828          </t>
+        </is>
+      </c>
+      <c r="K75" t="n">
+        <v>741.14</v>
+      </c>
+      <c r="L75" t="n">
+        <v>741.24</v>
+      </c>
+      <c r="M75" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>(-) de menos</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">862             </t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>J402111991</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>PIU EXPRESS, C.A.</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>10-10-2024</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>10002</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>00-00011343</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>11343</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>verificar n.control</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000633          </t>
+        </is>
+      </c>
+      <c r="K76" t="n">
+        <v>699.3099999999999</v>
+      </c>
+      <c r="L76" t="n">
+        <v>699.1799999999999</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>(+) de más</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">854             </t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>J405522194</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>CAFE EUROPA 2015, C.A.</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>03-10-2024</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>9867</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>00-00011208</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>00-00011208</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000407          </t>
+        </is>
+      </c>
+      <c r="K77" t="n">
+        <v>119.82</v>
+      </c>
+      <c r="L77" t="n">
+        <v>89.86</v>
+      </c>
+      <c r="M77" t="n">
+        <v>29.96</v>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>(+) de más</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">566             </t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>J406284513</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>NOSSO CAFE, C.A.</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>11-10-2024</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>10027</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>00-00011368</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>00-00011368</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000463          </t>
+        </is>
+      </c>
+      <c r="K78" t="n">
+        <v>121.99</v>
+      </c>
+      <c r="L78" t="n">
+        <v>121.99</v>
+      </c>
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>(-) de menos</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">848             </t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>J500533993</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>PANADERIA Y PASTELERIA TROPICAL PAN, C.A.</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>14-10-2024</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>10067</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>00-00011408</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>00-00011408</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000750          </t>
+        </is>
+      </c>
+      <c r="K79" t="n">
+        <v>722.96</v>
+      </c>
+      <c r="L79" t="n">
+        <v>722.97</v>
+      </c>
+      <c r="M79" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>(-) de menos</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">860             </t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>J500705050</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>INVERSIONES REGALEIRA, C.A.</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>30-09-2024</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>9773</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>00-00011114</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>00-00011114</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0000000497          </t>
+        </is>
+      </c>
+      <c r="K80" t="n">
+        <v>433.7</v>
+      </c>
+      <c r="L80" t="n">
+        <v>325.18</v>
+      </c>
+      <c r="M80" t="n">
+        <v>108.52</v>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>(+) de más</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
           <t xml:space="preserve">756             </t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C81" t="inlineStr">
         <is>
           <t>J502335803</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t>RENACER BAKERIES, C.A.</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>03-10-2024</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="F81" t="inlineStr">
         <is>
           <t>9866</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
+      <c r="G81" t="inlineStr">
         <is>
           <t>00-00011207</t>
         </is>
       </c>
-      <c r="H73" t="n">
+      <c r="H81" t="n">
         <v>11207</v>
       </c>
-      <c r="I73" t="inlineStr">
+      <c r="I81" t="inlineStr">
         <is>
           <t>verificar n.control</t>
         </is>
       </c>
-      <c r="J73" t="inlineStr">
+      <c r="J81" t="inlineStr">
         <is>
           <t xml:space="preserve">0000000430          </t>
         </is>
       </c>
-      <c r="K73" t="n">
+      <c r="K81" t="n">
         <v>292.11</v>
       </c>
-      <c r="L73" t="n">
+      <c r="L81" t="n">
         <v>219.29</v>
       </c>
-      <c r="M73" t="n">
+      <c r="M81" t="n">
         <v>72.81999999999999</v>
       </c>
-      <c r="N73" t="inlineStr">
+      <c r="N81" t="inlineStr">
         <is>
           <t>(+) de más</t>
         </is>

</xml_diff>